<commit_message>
Close loop Corrections PID corrections +DV value
</commit_message>
<xml_diff>
--- a/Data_step_response_MV.xlsx
+++ b/Data_step_response_MV.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\OneDrive - ECAM\Documents\Cours ECAM\4MIN\Q2 21-22\Control theory\2023\Laboratory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3E635F-EB6E-4B58-BA4D-10335CE8CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1108E01C-AF89-4ACD-A266-D1FDF22BA2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{799A8C1E-06C2-4169-9C7F-BECFFBB80892}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{799A8C1E-06C2-4169-9C7F-BECFFBB80892}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="MV" sheetId="1" r:id="rId1"/>
+    <sheet name="DV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
   <si>
     <t>KP</t>
   </si>
@@ -48,25 +49,34 @@
     <t>x</t>
   </si>
   <si>
-    <t>Numerical method 1st order (Broida) - MV Delta 20%</t>
+    <t>Theta</t>
   </si>
   <si>
-    <t>Numerical method 2nd order - MV Delta 20%</t>
+    <t>DV [%]</t>
   </si>
   <si>
-    <t>Numerical method 1st order - MV Delta 30%</t>
+    <t>Numerical method 1st order (Broida) - MV Delta 20% - DV 50%</t>
   </si>
   <si>
-    <t>Numerical method 2nd order - MV Delta 30%</t>
+    <t>Numerical method 2nd order - MV Delta 20% - DV 50%</t>
   </si>
   <si>
-    <t>Numerical method 1st order - MV Delta 40%</t>
+    <t>Numerical method 1st order - MV Delta 30% - DV 50%</t>
   </si>
   <si>
-    <t>Numerical method 2nd order - MV Delta 40%</t>
+    <t>Numerical method 2nd order - MV Delta 30% - DV 50%</t>
   </si>
   <si>
-    <t>Theta</t>
+    <t>Numerical method 1st order - MV Delta 40% - DV 50%</t>
+  </si>
+  <si>
+    <t>Numerical method 2nd order - MV Delta 40% - DV 50%</t>
+  </si>
+  <si>
+    <t>Numerical method 1st order (Broida) - DV Delta 20% - MV 50%</t>
+  </si>
+  <si>
+    <t>Numerical method 2nd order - DV Delta 20% - MV 50%</t>
   </si>
 </sst>
 </file>
@@ -321,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -387,6 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,7 +407,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +540,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$F$1</c:f>
+              <c:f>MV!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -550,7 +564,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$B$3:$F$3</c:f>
+              <c:f>MV!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -611,7 +625,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$C$1:$E$1</c:f>
+              <c:f>MV!$C$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -629,7 +643,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$12:$E$12</c:f>
+              <c:f>MV!$C$12:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -690,7 +704,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$D$1</c:f>
+              <c:f>MV!$D$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -702,7 +716,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$D$21</c:f>
+              <c:f>MV!$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1175,7 +1189,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$F$1</c:f>
+              <c:f>MV!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1199,7 +1213,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$B$4:$F$4</c:f>
+              <c:f>MV!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1260,7 +1274,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$C$1:$E$1</c:f>
+              <c:f>MV!$C$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1278,7 +1292,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$13:$E$13</c:f>
+              <c:f>MV!$C$13:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1333,7 +1347,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$D$1</c:f>
+              <c:f>MV!$D$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1345,7 +1359,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$D$22</c:f>
+              <c:f>MV!$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1820,7 +1834,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$F$1</c:f>
+              <c:f>MV!$B$1:$F$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1844,7 +1858,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$B$5:$F$5</c:f>
+              <c:f>MV!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1903,7 +1917,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$C$1:$E$1</c:f>
+              <c:f>MV!$C$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1921,7 +1935,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$14:$E$14</c:f>
+              <c:f>MV!$C$14:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1974,7 +1988,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$D$1</c:f>
+              <c:f>MV!$D$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1986,7 +2000,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$D$23</c:f>
+              <c:f>MV!$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -2333,6 +2347,1574 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>KP 1st order numericl method</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DV!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DV!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.39384830206558802</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48816890886234099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47934693115475602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38140120844895098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46089386327729998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-93CC-401C-B5F8-B49970AA9CD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>KP 2nd order numerical method</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DV!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DV!$B$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.32995934777097602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40629366537766398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47236626842657098</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37340705125976997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45821382709090602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-93CC-401C-B5F8-B49970AA9CD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="456799016"/>
+        <c:axId val="456799376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="456799016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456799376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="456799376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456799016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>T first order</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DV!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DV!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>188.31399553870199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227.736206702152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.86281536409101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>106.140557605579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>219.66622485606899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-85BB-48CF-A22D-556AE9172112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>T1 second order</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DV!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DV!$B$8:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>125.595657078987</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>147.818872494792</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>172.25941927414101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.079718976821596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215.172143681931</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-85BB-48CF-A22D-556AE9172112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>T2 second order</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DV!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DV!$B$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>23.237132717557198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.955610006673101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.150860875011698</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>12.7848633718881</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>12.220169759874899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-85BB-48CF-A22D-556AE9172112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="456784976"/>
+        <c:axId val="456785336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="456784976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456785336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="456785336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456784976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Theta 1st order</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DV!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DV!$B$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19.098713542278301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.0000138253702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.387701675067898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.184868427898898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.167720556635601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC71-440A-B561-322244C773AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Theta 2nd Order</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DV!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DV!$B$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.84895442810424</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.00001626057066</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53371654475178198</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6134662853492401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.45124843313751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CC71-440A-B561-322244C773AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="583835664"/>
+        <c:axId val="583824864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="583835664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583824864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="583824864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583835664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2453,6 +4035,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3486,6 +5188,1554 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4094,6 +7344,119 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2027815F-B1FE-D722-DE32-F0F2531AD2AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>745330</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>107155</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>745330</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>92868</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD837CF1-577F-0062-7D90-7765BA7B7F8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>573881</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>30956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>573881</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00C99178-DCC5-1DFA-9B18-BE9C4AF438A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>373856</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373856</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>40481</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6902A07-010D-FF47-235C-A4F54B30CFE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4413,8 +7776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4379861B-8E2C-4157-9800-1A920FC20378}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -4423,37 +7786,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="28">
+      <c r="B1" s="25">
         <v>30</v>
       </c>
-      <c r="C1" s="28">
+      <c r="C1" s="25">
         <v>40</v>
       </c>
-      <c r="D1" s="28">
+      <c r="D1" s="25">
         <v>50</v>
       </c>
-      <c r="E1" s="28">
+      <c r="E1" s="25">
         <v>60</v>
       </c>
-      <c r="F1" s="28">
+      <c r="F1" s="25">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A2" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
+      <c r="A2" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="15">
@@ -4473,7 +7836,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="16">
@@ -4493,8 +7856,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A5" s="28" t="s">
-        <v>13</v>
+      <c r="A5" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="16">
         <v>0.18419198211416701</v>
@@ -4513,17 +7876,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A6" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
+      <c r="A6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="17" t="s">
@@ -4543,7 +7906,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -4563,7 +7926,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -4583,8 +7946,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A10" s="28" t="s">
-        <v>13</v>
+      <c r="A10" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>4</v>
@@ -4603,17 +7966,17 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A11" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
+      <c r="A11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -4633,7 +7996,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -4653,8 +8016,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A14" s="28" t="s">
-        <v>13</v>
+      <c r="A14" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>6</v>
@@ -4673,23 +8036,25 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
     </row>
     <row r="16" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="D16" s="8" t="s">
         <v>4</v>
       </c>
@@ -4701,13 +8066,15 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
@@ -4719,13 +8086,15 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
@@ -4737,13 +8106,15 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A19" s="28" t="s">
-        <v>13</v>
+      <c r="A19" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>4</v>
       </c>
@@ -4755,17 +8126,17 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A20" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
+      <c r="A20" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
     </row>
     <row r="21" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -4785,7 +8156,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="20" t="s">
@@ -4805,8 +8176,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A23" s="28" t="s">
-        <v>13</v>
+      <c r="A23" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>6</v>
@@ -4825,17 +8196,17 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A24" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="27"/>
+      <c r="A24" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -4855,7 +8226,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -4875,7 +8246,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="20" t="s">
@@ -4895,8 +8266,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.65" thickBot="1">
-      <c r="A28" s="28" t="s">
-        <v>13</v>
+      <c r="A28" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>6</v>
@@ -4927,4 +8298,205 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA794C66-31D0-4430-98BA-175676365801}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="25">
+        <v>30</v>
+      </c>
+      <c r="C1" s="25">
+        <v>40</v>
+      </c>
+      <c r="D1" s="25">
+        <v>50</v>
+      </c>
+      <c r="E1" s="25">
+        <v>60</v>
+      </c>
+      <c r="F1" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A2" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0.39384830206558802</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.48816890886234099</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.47934693115475602</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.38140120844895098</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.46089386327729998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A4" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16">
+        <v>188.31399553870199</v>
+      </c>
+      <c r="C4" s="2">
+        <v>227.736206702152</v>
+      </c>
+      <c r="D4" s="2">
+        <v>183.86281536409101</v>
+      </c>
+      <c r="E4" s="2">
+        <v>106.140557605579</v>
+      </c>
+      <c r="F4" s="4">
+        <v>219.66622485606899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A5" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16">
+        <v>19.098713542278301</v>
+      </c>
+      <c r="C5" s="2">
+        <v>17.0000138253702</v>
+      </c>
+      <c r="D5" s="29">
+        <v>18.387701675067898</v>
+      </c>
+      <c r="E5" s="2">
+        <v>16.184868427898898</v>
+      </c>
+      <c r="F5" s="4">
+        <v>13.167720556635601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A7" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="29">
+        <v>0.32995934777097602</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.40629366537766398</v>
+      </c>
+      <c r="D7" s="29">
+        <v>0.47236626842657098</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0.37340705125976997</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.45821382709090602</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>125.595657078987</v>
+      </c>
+      <c r="C8" s="2">
+        <v>147.818872494792</v>
+      </c>
+      <c r="D8" s="2">
+        <v>172.25941927414101</v>
+      </c>
+      <c r="E8" s="2">
+        <v>96.079718976821596</v>
+      </c>
+      <c r="F8" s="4">
+        <v>215.172143681931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A9" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>23.237132717557198</v>
+      </c>
+      <c r="C9" s="2">
+        <v>30.955610006673101</v>
+      </c>
+      <c r="D9" s="2">
+        <v>22.150860875011698</v>
+      </c>
+      <c r="E9" s="3">
+        <v>12.7848633718881</v>
+      </c>
+      <c r="F9" s="5">
+        <v>12.220169759874899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A10" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="18">
+        <v>7.84895442810424</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.00001626057066</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.53371654475178198</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6.6134662853492401</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2.45124843313751</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>